<commit_message>
start telegram bot and add umarbek referrals
</commit_message>
<xml_diff>
--- a/shop_daily_report.xlsx
+++ b/shop_daily_report.xlsx
@@ -482,19 +482,19 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B2" t="n">
         <v>105815</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>4244.333333333334</v>
       </c>
       <c r="D2" t="n">
         <v>4325</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>117666.6666666667</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
@@ -503,7 +503,7 @@
         <v>4.9</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>5761</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>

</xml_diff>